<commit_message>
still going through edits
</commit_message>
<xml_diff>
--- a/SOSPaper/Tables_SOS.xlsx
+++ b/SOSPaper/Tables_SOS.xlsx
@@ -927,7 +927,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1041,7 +1041,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1341,7 +1340,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:O7"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1368,7 +1367,7 @@
     <col min="21" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="12.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>6.2953239999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
         <v>27</v>
       </c>
@@ -1743,7 +1742,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
         <v>11</v>
       </c>
@@ -1759,7 +1758,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
         <v>7</v>
       </c>
@@ -1767,7 +1766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>2</v>
       </c>
@@ -1776,14 +1775,14 @@
       </c>
       <c r="C15" s="35"/>
     </row>
-    <row r="16" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
     </row>
-    <row r="17" spans="1:3" ht="12.95" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
         <v>3</v>
       </c>
@@ -1792,14 +1791,14 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="35"/>
       <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="12.95" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
         <v>1</v>
       </c>
@@ -1817,12 +1816,12 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>58</v>
       </c>
@@ -1841,29 +1840,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:G28"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" style="3" customWidth="1"/>
     <col min="2" max="2" width="58.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -1886,7 +1884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>42</v>
       </c>
@@ -1897,7 +1895,7 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1920,7 +1918,7 @@
         <v>2007000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -2035,13 +2033,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>177</v>
       </c>
       <c r="B10" s="27"/>
     </row>
-    <row r="11" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
@@ -2064,7 +2062,7 @@
         <v>0.61470000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -2087,7 +2085,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>97</v>
       </c>
@@ -2133,7 +2131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -2179,7 +2177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>98</v>
       </c>
@@ -2202,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>176</v>
       </c>
@@ -2254,7 +2252,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>90</v>
       </c>
@@ -2277,13 +2275,13 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="27"/>
     </row>
-    <row r="23" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
         <v>116</v>
       </c>
@@ -2306,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>117</v>
       </c>
@@ -2349,13 +2347,13 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="32"/>
     </row>
-    <row r="27" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>142</v>
       </c>
@@ -2383,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>141</v>
       </c>
@@ -2409,6 +2407,40 @@
       <c r="G28" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="29">
+        <v>713800</v>
+      </c>
+      <c r="D37" s="29">
+        <v>13260000</v>
+      </c>
+      <c r="E37" s="29">
+        <v>1490000</v>
+      </c>
+      <c r="F37" s="29">
+        <v>16079000</v>
+      </c>
+      <c r="G37" s="29">
+        <v>5650000000</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C38" s="29">
+        <v>8320000</v>
+      </c>
+      <c r="D38" s="29">
+        <v>110000000</v>
+      </c>
+      <c r="E38" s="29">
+        <v>10566000</v>
+      </c>
+      <c r="F38" s="29">
+        <v>234753400</v>
+      </c>
+      <c r="G38" s="29">
+        <v>153000000000</v>
       </c>
     </row>
   </sheetData>
@@ -2433,351 +2465,351 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="56" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="57" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="57" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="55" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="55" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="55" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="56"/>
+      <c r="C16" s="55"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="56"/>
+      <c r="C17" s="55"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="56"/>
+      <c r="C18" s="55"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="56"/>
+      <c r="C19" s="55"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="55" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="55" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="56"/>
+      <c r="C21" s="55"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="56"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="55"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="56"/>
+      <c r="C23" s="55"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="55" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="56"/>
+      <c r="C24" s="55"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="56"/>
+      <c r="C25" s="55"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="56"/>
+      <c r="C26" s="55"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="56"/>
+      <c r="C27" s="55"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="56"/>
+      <c r="C28" s="55"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="56"/>
+      <c r="C29" s="55"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="56"/>
+      <c r="C30" s="55"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="56"/>
+      <c r="C32" s="55"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="C33" s="56"/>
+      <c r="C33" s="55"/>
     </row>
     <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="C34" s="56"/>
+      <c r="C34" s="55"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="60" t="s">
+      <c r="A35" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="60"/>
-      <c r="C35" s="56"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="55"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="60" t="s">
+      <c r="A36" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="60"/>
-      <c r="C36" s="56"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="55"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="62" t="s">
+      <c r="A37" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2864,19 +2896,19 @@
       <c r="B7" s="26">
         <v>0.73</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="54">
         <v>0.96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>126</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="53" t="s">
         <v>125</v>
       </c>
       <c r="B9" s="3"/>
@@ -2893,14 +2925,15 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="9.140625" style="3"/>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" customWidth="1"/>
+    <col min="6" max="16" width="9.140625" style="3"/>
     <col min="17" max="17" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="3"/>
@@ -2928,22 +2961,22 @@
         <v>62</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>61</v>
@@ -2981,25 +3014,25 @@
         <v>32.030085938262403</v>
       </c>
       <c r="D3" s="36">
-        <v>-47.460396897583202</v>
-      </c>
-      <c r="E3" s="36">
-        <v>-5.3015735441525198</v>
-      </c>
-      <c r="F3" s="36">
-        <f>D3-E3</f>
-        <v>-42.158823353430684</v>
-      </c>
-      <c r="G3" s="36">
-        <v>-17.604515027533399</v>
-      </c>
-      <c r="H3" s="36">
         <f>SUM(B3:C3)</f>
         <v>71.914353690444699</v>
       </c>
+      <c r="E3" s="36">
+        <f>D3-ABS(I3)</f>
+        <v>54.309838662911304</v>
+      </c>
+      <c r="F3" s="36">
+        <v>-47.460396897583202</v>
+      </c>
+      <c r="G3" s="36">
+        <v>-5.3015735441525198</v>
+      </c>
+      <c r="H3" s="36">
+        <f>G3-F3</f>
+        <v>42.158823353430684</v>
+      </c>
       <c r="I3" s="36">
-        <f>H3+G3</f>
-        <v>54.309838662911304</v>
+        <v>-17.604515027533399</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>5</v>
@@ -3034,25 +3067,25 @@
         <v>54.2279097996581</v>
       </c>
       <c r="D4" s="36">
+        <f t="shared" ref="D4:D7" si="0">SUM(B4:C4)</f>
+        <v>118.97153169201809</v>
+      </c>
+      <c r="E4" s="36">
+        <f t="shared" ref="E4:E7" si="1">D4-ABS(I4)</f>
+        <v>59.023105742663191</v>
+      </c>
+      <c r="F4" s="36">
         <v>-16.7559221505552</v>
       </c>
-      <c r="E4" s="36">
+      <c r="G4" s="36">
         <v>-43.810372814785403</v>
       </c>
-      <c r="F4" s="36">
-        <f t="shared" ref="F4:F7" si="0">D4-E4</f>
-        <v>27.054450664230203</v>
-      </c>
-      <c r="G4" s="36">
+      <c r="H4" s="36">
+        <f t="shared" ref="H4:H7" si="2">G4-F4</f>
+        <v>-27.054450664230203</v>
+      </c>
+      <c r="I4" s="36">
         <v>-59.948425949354899</v>
-      </c>
-      <c r="H4" s="36">
-        <f t="shared" ref="H4:H7" si="1">SUM(B4:C4)</f>
-        <v>118.97153169201809</v>
-      </c>
-      <c r="I4" s="36">
-        <f t="shared" ref="I4:I7" si="2">H4+G4</f>
-        <v>59.023105742663191</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>58</v>
@@ -3069,25 +3102,25 @@
         <v>11.2676861219134</v>
       </c>
       <c r="D5" s="36">
+        <f t="shared" si="0"/>
+        <v>87.452850307993501</v>
+      </c>
+      <c r="E5" s="36">
+        <f t="shared" si="1"/>
+        <v>31.861276174582798</v>
+      </c>
+      <c r="F5" s="36">
         <v>-23.679601554151802</v>
       </c>
-      <c r="E5" s="36">
+      <c r="G5" s="36">
         <v>-6.6698056854628902</v>
       </c>
-      <c r="F5" s="36">
-        <f t="shared" si="0"/>
-        <v>-17.009795868688911</v>
-      </c>
-      <c r="G5" s="36">
+      <c r="H5" s="36">
+        <f t="shared" si="2"/>
+        <v>17.009795868688911</v>
+      </c>
+      <c r="I5" s="36">
         <v>-55.591574133410703</v>
-      </c>
-      <c r="H5" s="36">
-        <f t="shared" si="1"/>
-        <v>87.452850307993501</v>
-      </c>
-      <c r="I5" s="36">
-        <f t="shared" si="2"/>
-        <v>31.861276174582798</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>3</v>
@@ -3104,25 +3137,25 @@
         <v>28.166097455548801</v>
       </c>
       <c r="D6" s="36">
+        <f t="shared" si="0"/>
+        <v>41.517021796786302</v>
+      </c>
+      <c r="E6" s="36">
+        <f t="shared" si="1"/>
+        <v>37.562873911374481</v>
+      </c>
+      <c r="F6" s="36">
         <v>-37.449702400323901</v>
       </c>
-      <c r="E6" s="36">
+      <c r="G6" s="36">
         <v>-1.19484799052451</v>
       </c>
-      <c r="F6" s="36">
-        <f t="shared" si="0"/>
-        <v>-36.254854409799393</v>
-      </c>
-      <c r="G6" s="36">
+      <c r="H6" s="36">
+        <f t="shared" si="2"/>
+        <v>36.254854409799393</v>
+      </c>
+      <c r="I6" s="36">
         <v>-3.9541478854118202</v>
-      </c>
-      <c r="H6" s="36">
-        <f t="shared" si="1"/>
-        <v>41.517021796786302</v>
-      </c>
-      <c r="I6" s="36">
-        <f t="shared" si="2"/>
-        <v>37.562873911374481</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>1</v>
@@ -3151,39 +3184,39 @@
       <c r="A7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="36">
         <v>32.246509970924897</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="36">
         <v>26.076400766691801</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="36">
+        <f t="shared" si="0"/>
+        <v>58.322910737616695</v>
+      </c>
+      <c r="E7" s="36">
+        <f t="shared" si="1"/>
+        <v>46.200434600374095</v>
+      </c>
+      <c r="F7" s="36">
         <v>-29.199450934017602</v>
       </c>
-      <c r="E7" s="3">
+      <c r="G7" s="36">
         <v>-19.850623668752998</v>
       </c>
-      <c r="F7" s="36">
-        <f t="shared" si="0"/>
-        <v>-9.3488272652646032</v>
-      </c>
-      <c r="G7" s="36">
+      <c r="H7" s="36">
+        <f t="shared" si="2"/>
+        <v>9.3488272652646032</v>
+      </c>
+      <c r="I7" s="36">
         <v>-12.1224761372426</v>
-      </c>
-      <c r="H7" s="53">
-        <f t="shared" si="1"/>
-        <v>58.322910737616695</v>
-      </c>
-      <c r="I7" s="36">
-        <f t="shared" si="2"/>
-        <v>46.200434600374095</v>
       </c>
       <c r="K7" s="33" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F8" s="36"/>
+      <c r="H8" s="36"/>
     </row>
     <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
@@ -3193,8 +3226,10 @@
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
-      <c r="F9" s="36"/>
+      <c r="F9"/>
       <c r="G9"/>
+      <c r="H9" s="36"/>
+      <c r="I9"/>
       <c r="K9" s="52" t="s">
         <v>122</v>
       </c>
@@ -3205,29 +3240,36 @@
         <v>5</v>
       </c>
       <c r="B10" s="36">
-        <f>B3/$H$3</f>
+        <f>B3/D3</f>
         <v>0.55460788709669995</v>
       </c>
       <c r="C10" s="36">
-        <f t="shared" ref="C10:G10" si="3">C3/$H$3</f>
+        <f>C3/D3</f>
         <v>0.44539211290330011</v>
       </c>
       <c r="D10" s="36">
-        <f>D3/$H$3</f>
+        <f>SUM(B10:C10)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="36">
+        <f>E3/D3</f>
+        <v>0.75520165135166173</v>
+      </c>
+      <c r="F10" s="36">
+        <f>F3/D3</f>
         <v>-0.65995721941514562</v>
       </c>
-      <c r="E10" s="36">
-        <f t="shared" si="3"/>
+      <c r="G10" s="36">
+        <f>G3/D3</f>
         <v>-7.3720658979612622E-2</v>
       </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36">
-        <f t="shared" si="3"/>
+      <c r="H10" s="36">
+        <f>H3/D3</f>
+        <v>0.58623656043553307</v>
+      </c>
+      <c r="I10" s="36">
+        <f>I3/D3</f>
         <v>-0.24479834864833835</v>
-      </c>
-      <c r="I10" s="3">
-        <f>I3/H3</f>
-        <v>0.75520165135166173</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>5</v>
@@ -3238,29 +3280,36 @@
         <v>58</v>
       </c>
       <c r="B11" s="36">
-        <f>B4/$H$4</f>
+        <f t="shared" ref="B11:B14" si="3">B4/D4</f>
         <v>0.54419423681929202</v>
       </c>
       <c r="C11" s="36">
-        <f t="shared" ref="C11:G11" si="4">C4/$H$4</f>
+        <f t="shared" ref="C11:C14" si="4">C4/D4</f>
         <v>0.45580576318070803</v>
       </c>
       <c r="D11" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D11:D14" si="5">SUM(B11:C11)</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="36">
+        <f>E4/D4</f>
+        <v>0.49611116964902541</v>
+      </c>
+      <c r="F11" s="36">
+        <f t="shared" ref="F11:F14" si="6">F4/D4</f>
         <v>-0.14083976151480759</v>
       </c>
-      <c r="E11" s="36">
-        <f t="shared" si="4"/>
+      <c r="G11" s="36">
+        <f t="shared" ref="G11:G14" si="7">G4/D4</f>
         <v>-0.36824248786001534</v>
       </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36">
-        <f t="shared" si="4"/>
+      <c r="H11" s="36">
+        <f t="shared" ref="H11:H14" si="8">H4/D4</f>
+        <v>-0.22740272634520775</v>
+      </c>
+      <c r="I11" s="36">
+        <f t="shared" ref="I11:I14" si="9">I4/D4</f>
         <v>-0.50388883035097454</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" ref="I11:I14" si="5">I4/H4</f>
-        <v>0.49611116964902541</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>58</v>
@@ -3271,29 +3320,36 @@
         <v>3</v>
       </c>
       <c r="B12" s="36">
-        <f>B5/$H$5</f>
+        <f t="shared" si="3"/>
         <v>0.87115701681270996</v>
       </c>
       <c r="C12" s="36">
-        <f t="shared" ref="C12:G12" si="6">C5/$H$5</f>
+        <f t="shared" si="4"/>
         <v>0.12884298318729004</v>
       </c>
       <c r="D12" s="36">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="36">
+        <f t="shared" ref="E12:E14" si="10">E5/D5</f>
+        <v>0.3643251885144167</v>
+      </c>
+      <c r="F12" s="36">
         <f t="shared" si="6"/>
         <v>-0.27076992311578668</v>
       </c>
-      <c r="E12" s="36">
-        <f t="shared" si="6"/>
+      <c r="G12" s="36">
+        <f t="shared" si="7"/>
         <v>-7.6267447681499373E-2</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36">
-        <f t="shared" si="6"/>
+      <c r="H12" s="36">
+        <f t="shared" si="8"/>
+        <v>0.19450247543428731</v>
+      </c>
+      <c r="I12" s="36">
+        <f t="shared" si="9"/>
         <v>-0.63567481148558325</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" si="5"/>
-        <v>0.3643251885144167</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>3</v>
@@ -3313,29 +3369,36 @@
         <v>1</v>
       </c>
       <c r="B13" s="36">
-        <f>B6/$H$6</f>
+        <f t="shared" si="3"/>
         <v>0.32157712098392738</v>
       </c>
       <c r="C13" s="36">
-        <f t="shared" ref="C13:G13" si="7">C6/$H$6</f>
+        <f t="shared" si="4"/>
         <v>0.67842287901607257</v>
       </c>
       <c r="D13" s="36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="36">
+        <f t="shared" si="10"/>
+        <v>0.90475839271982894</v>
+      </c>
+      <c r="F13" s="36">
+        <f t="shared" si="6"/>
         <v>-0.90203248642518863</v>
       </c>
-      <c r="E13" s="36">
+      <c r="G13" s="36">
         <f t="shared" si="7"/>
         <v>-2.8779713447967002E-2</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36">
-        <f t="shared" si="7"/>
+      <c r="H13" s="36">
+        <f t="shared" si="8"/>
+        <v>0.8732527729772217</v>
+      </c>
+      <c r="I13" s="36">
+        <f t="shared" si="9"/>
         <v>-9.524160728017099E-2</v>
-      </c>
-      <c r="I13" s="3">
-        <f t="shared" si="5"/>
-        <v>0.90475839271982894</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>1</v>
@@ -3358,34 +3421,43 @@
         <v>4</v>
       </c>
       <c r="B14" s="37">
-        <f>B7/$H$7</f>
+        <f t="shared" si="3"/>
         <v>0.55289610143080137</v>
       </c>
       <c r="C14" s="37">
-        <f t="shared" ref="C14:G14" si="8">C7/$H$7</f>
+        <f t="shared" si="4"/>
         <v>0.44710389856919863</v>
       </c>
       <c r="D14" s="37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="37">
+        <f t="shared" si="10"/>
+        <v>0.79214898598289729</v>
+      </c>
+      <c r="F14" s="37">
+        <f t="shared" si="6"/>
+        <v>-0.50065146894640067</v>
+      </c>
+      <c r="G14" s="37">
+        <f t="shared" si="7"/>
+        <v>-0.34035721841896832</v>
+      </c>
+      <c r="H14" s="37">
         <f t="shared" si="8"/>
-        <v>-0.50065146894640067</v>
-      </c>
-      <c r="E14" s="37">
-        <f t="shared" si="8"/>
-        <v>-0.34035721841896832</v>
-      </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37">
-        <f t="shared" si="8"/>
+        <v>0.16029425052743232</v>
+      </c>
+      <c r="I14" s="37">
+        <f t="shared" si="9"/>
         <v>-0.20785101401710276</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="3">
-        <f t="shared" si="5"/>
-        <v>0.79214898598289729</v>
       </c>
       <c r="K14" s="26" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="29"/>
     </row>
     <row r="37" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
new fits and results
</commit_message>
<xml_diff>
--- a/SOSPaper/Tables_SOS.xlsx
+++ b/SOSPaper/Tables_SOS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ian_GIS\gleon\SOS\SOSPaper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hilarydugan/Documents/SOS/SOSPaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2578033C-10F0-BB40-8C8C-43A553C5F9A2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22920" windowHeight="16780" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="4) Model fits" sheetId="5" r:id="rId4"/>
     <sheet name="5) Mass balances" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="185">
   <si>
     <t>Lake</t>
   </si>
@@ -774,11 +775,14 @@
   <si>
     <t>Standard deviation of annual means</t>
   </si>
+  <si>
+    <t>&lt;-- Updated May 8 2018 HD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1343,43 +1347,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" style="3"/>
-    <col min="20" max="20" width="8.5703125" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="8.85546875" style="3"/>
+    <col min="5" max="5" width="6.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="8.5" style="3" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" style="3"/>
+    <col min="20" max="20" width="8.5" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="12" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="12" customFormat="1" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1441,7 +1445,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1503,7 +1507,7 @@
         <v>6.2953239999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -1557,7 +1561,7 @@
         <v>135.56549999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
@@ -1619,7 +1623,7 @@
         <v>3.787623</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="26.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1681,7 +1685,7 @@
         <v>10.98129</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
@@ -1735,12 +1739,12 @@
         <v>6.2953239999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10" s="34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11" s="35" t="s">
         <v>6</v>
       </c>
@@ -1749,14 +1753,14 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13" s="35" t="s">
         <v>5</v>
       </c>
@@ -1765,7 +1769,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14" s="35" t="s">
         <v>7</v>
       </c>
@@ -1773,7 +1777,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15" s="35" t="s">
         <v>2</v>
       </c>
@@ -1782,14 +1786,14 @@
       </c>
       <c r="C15" s="35"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="35" t="s">
         <v>3</v>
       </c>
@@ -1798,14 +1802,14 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="35"/>
       <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="35" t="s">
         <v>1</v>
       </c>
@@ -1814,7 +1818,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="35" t="s">
         <v>4</v>
       </c>
@@ -1823,12 +1827,12 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
         <v>58</v>
       </c>
@@ -1838,7 +1842,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1"/>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1846,29 +1850,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25" style="3" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -1891,7 +1895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="27" t="s">
         <v>42</v>
       </c>
@@ -1902,7 +1906,7 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>2007000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1948,7 +1952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>75</v>
       </c>
@@ -1971,7 +1975,7 @@
         <v>5650000000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1994,7 +1998,7 @@
         <v>153000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>76</v>
       </c>
@@ -2017,7 +2021,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -2040,13 +2044,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="27" t="s">
         <v>177</v>
       </c>
       <c r="B10" s="27"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
@@ -2069,7 +2073,7 @@
         <v>0.61470000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -2092,7 +2096,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>97</v>
       </c>
@@ -2115,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>78</v>
       </c>
@@ -2138,7 +2142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -2161,7 +2165,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
@@ -2184,7 +2188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>98</v>
       </c>
@@ -2207,13 +2211,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="27" t="s">
         <v>176</v>
       </c>
       <c r="B18" s="27"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>145</v>
       </c>
@@ -2236,7 +2240,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="30" t="s">
         <v>146</v>
       </c>
@@ -2259,7 +2263,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>90</v>
       </c>
@@ -2282,13 +2286,13 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="27" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="27"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="30" t="s">
         <v>116</v>
       </c>
@@ -2311,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="30" t="s">
         <v>117</v>
       </c>
@@ -2334,7 +2338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>77</v>
       </c>
@@ -2354,13 +2358,13 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="32"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>142</v>
       </c>
@@ -2388,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
         <v>141</v>
       </c>
@@ -2416,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C37" s="29">
         <v>713800</v>
       </c>
@@ -2433,7 +2437,7 @@
         <v>5650000000</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C38" s="29">
         <v>8320000</v>
       </c>
@@ -2457,28 +2461,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="97.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="97.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>72</v>
       </c>
       <c r="B1" s="55"/>
       <c r="C1" s="55"/>
     </row>
-    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>166</v>
       </c>
@@ -2489,7 +2493,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
         <v>155</v>
       </c>
@@ -2500,7 +2504,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="57" t="s">
         <v>156</v>
       </c>
@@ -2511,7 +2515,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
         <v>157</v>
       </c>
@@ -2522,7 +2526,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="57" t="s">
         <v>158</v>
       </c>
@@ -2533,7 +2537,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
         <v>159</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="57" t="s">
         <v>160</v>
       </c>
@@ -2555,7 +2559,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="57" t="s">
         <v>161</v>
       </c>
@@ -2566,7 +2570,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="57" t="s">
         <v>162</v>
       </c>
@@ -2577,7 +2581,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="57" t="s">
         <v>163</v>
       </c>
@@ -2588,7 +2592,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
         <v>167</v>
       </c>
@@ -2599,14 +2603,14 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="58" t="s">
         <v>168</v>
       </c>
       <c r="B13" s="55"/>
       <c r="C13" s="55"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="57" t="s">
         <v>127</v>
       </c>
@@ -2617,7 +2621,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="57" t="s">
         <v>128</v>
       </c>
@@ -2628,7 +2632,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="s">
         <v>129</v>
       </c>
@@ -2637,7 +2641,7 @@
       </c>
       <c r="C16" s="55"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="55" t="s">
         <v>130</v>
       </c>
@@ -2646,7 +2650,7 @@
       </c>
       <c r="C17" s="55"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="55" t="s">
         <v>131</v>
       </c>
@@ -2655,7 +2659,7 @@
       </c>
       <c r="C18" s="55"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="55" t="s">
         <v>132</v>
       </c>
@@ -2664,7 +2668,7 @@
       </c>
       <c r="C19" s="55"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
         <v>133</v>
       </c>
@@ -2675,7 +2679,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="55" t="s">
         <v>134</v>
       </c>
@@ -2684,14 +2688,14 @@
       </c>
       <c r="C21" s="55"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="58" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="58"/>
       <c r="C22" s="55"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="55" t="s">
         <v>135</v>
       </c>
@@ -2700,7 +2704,7 @@
       </c>
       <c r="C23" s="55"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
         <v>164</v>
       </c>
@@ -2709,7 +2713,7 @@
       </c>
       <c r="C24" s="55"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="55" t="s">
         <v>165</v>
       </c>
@@ -2718,7 +2722,7 @@
       </c>
       <c r="C25" s="55"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="55" t="s">
         <v>136</v>
       </c>
@@ -2727,7 +2731,7 @@
       </c>
       <c r="C26" s="55"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="55" t="s">
         <v>169</v>
       </c>
@@ -2736,7 +2740,7 @@
       </c>
       <c r="C27" s="55"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="55" t="s">
         <v>170</v>
       </c>
@@ -2745,7 +2749,7 @@
       </c>
       <c r="C28" s="55"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="55" t="s">
         <v>171</v>
       </c>
@@ -2754,7 +2758,7 @@
       </c>
       <c r="C29" s="55"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="59" t="s">
         <v>172</v>
       </c>
@@ -2763,14 +2767,14 @@
       </c>
       <c r="C30" s="55"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="58" t="s">
         <v>93</v>
       </c>
       <c r="B31" s="55"/>
       <c r="C31" s="55"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="55" t="s">
         <v>137</v>
       </c>
@@ -2779,7 +2783,7 @@
       </c>
       <c r="C32" s="55"/>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="55" t="s">
         <v>138</v>
       </c>
@@ -2788,7 +2792,7 @@
       </c>
       <c r="C33" s="55"/>
     </row>
-    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="60" t="s">
         <v>139</v>
       </c>
@@ -2797,21 +2801,21 @@
       </c>
       <c r="C34" s="55"/>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="59" t="s">
         <v>107</v>
       </c>
       <c r="B35" s="59"/>
       <c r="C35" s="55"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="59" t="s">
         <v>140</v>
       </c>
       <c r="B36" s="59"/>
       <c r="C36" s="55"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="61" t="s">
         <v>173</v>
       </c>
@@ -2825,23 +2829,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="A1:C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>178</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2851,8 +2858,20 @@
       <c r="C2" s="6" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2862,8 +2881,17 @@
       <c r="C3" s="50">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1.2488489306156501</v>
+      </c>
+      <c r="H3">
+        <v>0.85389351218815102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -2873,8 +2901,17 @@
       <c r="C4" s="50">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4">
+        <v>1.4641714180909799</v>
+      </c>
+      <c r="H4">
+        <v>0.69837503040359505</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2884,8 +2921,17 @@
       <c r="C5" s="50">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>1.2123881443494</v>
+      </c>
+      <c r="H5">
+        <v>0.79254393893729602</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -2895,8 +2941,17 @@
       <c r="C6" s="50">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.80209904665356302</v>
+      </c>
+      <c r="H6">
+        <v>0.95158047733254303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
@@ -2906,20 +2961,35 @@
       <c r="C7" s="54">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>0.72408838354316896</v>
+      </c>
+      <c r="H7">
+        <v>0.965139555519964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="53" t="s">
         <v>126</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" s="53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>125</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
+      <c r="F9" s="53" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2928,27 +2998,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" customWidth="1"/>
-    <col min="6" max="16" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.1640625" style="3"/>
+    <col min="2" max="2" width="19.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="3"/>
+    <col min="4" max="4" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="3" customWidth="1"/>
+    <col min="6" max="16" width="9.1640625" style="3"/>
     <col min="17" max="17" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="3"/>
+    <col min="18" max="18" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>181</v>
       </c>
@@ -2959,7 +3029,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -3012,7 +3082,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="52" t="s">
         <v>182</v>
       </c>
@@ -3038,7 +3108,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3073,7 +3143,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>58</v>
       </c>
@@ -3108,7 +3178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -3162,7 +3232,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -3197,7 +3267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>4</v>
       </c>
@@ -3229,7 +3299,7 @@
         <v>-12.1224761372426</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="52" t="s">
         <v>183</v>
       </c>
@@ -3246,7 +3316,7 @@
       </c>
       <c r="L9" s="52"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -3278,7 +3348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
@@ -3310,7 +3380,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -3351,7 +3421,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -3395,7 +3465,7 @@
         <v>0.31092964824120606</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
         <v>4</v>
       </c>
@@ -3427,7 +3497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="52" t="s">
         <v>122</v>
       </c>
@@ -3440,7 +3510,7 @@
       <c r="H15" s="50"/>
       <c r="I15" s="62"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -3477,7 +3547,7 @@
         <v>-0.24479834864833835</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
@@ -3514,7 +3584,7 @@
         <v>-0.50388883035097454</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -3551,7 +3621,7 @@
         <v>-0.63567481148558325</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
@@ -3588,7 +3658,7 @@
         <v>-9.524160728017099E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>4</v>
       </c>
@@ -3625,7 +3695,7 @@
         <v>-0.20785101401710276</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
       <c r="D21" s="50"/>
@@ -3635,7 +3705,7 @@
       <c r="H21" s="50"/>
       <c r="I21" s="50"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B22" s="50"/>
       <c r="C22" s="50"/>
       <c r="D22" s="50"/>
@@ -3645,7 +3715,7 @@
       <c r="H22" s="50"/>
       <c r="I22" s="50"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
@@ -3655,7 +3725,7 @@
       <c r="H23" s="50"/>
       <c r="I23" s="50"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="50"/>
       <c r="C24" s="50"/>
       <c r="D24" s="50"/>
@@ -3665,7 +3735,7 @@
       <c r="H24" s="50"/>
       <c r="I24" s="50"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
@@ -3675,7 +3745,7 @@
       <c r="H25" s="50"/>
       <c r="I25" s="50"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
@@ -3685,7 +3755,7 @@
       <c r="H26" s="50"/>
       <c r="I26" s="50"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="33"/>
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
@@ -3696,7 +3766,7 @@
       <c r="H27" s="50"/>
       <c r="I27" s="50"/>
     </row>
-    <row r="37" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="8.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>